<commit_message>
try to fix unresolved test
</commit_message>
<xml_diff>
--- a/test/module-xlsx/table.xlsx
+++ b/test/module-xlsx/table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>on</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>k3</t>
+  </si>
+  <si>
+    <t>waitSec</t>
   </si>
 </sst>
 </file>
@@ -438,7 +441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -558,15 +561,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -585,8 +588,11 @@
       <c r="F1" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -604,6 +610,9 @@
       </c>
       <c r="F2">
         <v>1</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change container structure - add namespace class - remove storage class - update tests - rename populate to knit - add requirements of setNS - temporally remove import
</commit_message>
<xml_diff>
--- a/test/module-xlsx/table.xlsx
+++ b/test/module-xlsx/table.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
   <si>
     <t>on</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>k6</t>
+  </si>
+  <si>
+    <t>setNS</t>
   </si>
 </sst>
 </file>
@@ -460,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -507,40 +510,22 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
       </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4">
-        <v>1.2</v>
-      </c>
-      <c r="H4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -552,7 +537,7 @@
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="G5">
         <v>1.2</v>
@@ -563,10 +548,13 @@
       <c r="I5" t="s">
         <v>15</v>
       </c>
+      <c r="K5" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -574,46 +562,72 @@
       <c r="D6" t="s">
         <v>9</v>
       </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G6">
         <v>1.2</v>
       </c>
-      <c r="K6" t="s">
-        <v>28</v>
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
       <c r="F7" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>1.2</v>
+      </c>
+      <c r="K7" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
-        <v>30</v>
+      <c r="B8">
+        <v>2</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
+        <v>29</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
       <c r="F9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
allow 0/1 as boolean imn table
</commit_message>
<xml_diff>
--- a/test/module-xlsx/table.xlsx
+++ b/test/module-xlsx/table.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
   <si>
     <t>on</t>
   </si>
@@ -118,6 +118,24 @@
   </si>
   <si>
     <t>setNS</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>s1</t>
+  </si>
+  <si>
+    <t>isAmount</t>
+  </si>
+  <si>
+    <t>Compartment</t>
+  </si>
+  <si>
+    <t>compartment</t>
+  </si>
+  <si>
+    <t>c1</t>
   </si>
 </sst>
 </file>
@@ -463,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -477,7 +495,7 @@
     <col min="10" max="10" width="19.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -508,8 +526,14 @@
       <c r="K1" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>1</v>
       </c>
@@ -520,7 +544,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -552,7 +576,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>0</v>
       </c>
@@ -578,7 +602,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B7">
         <v>1</v>
       </c>
@@ -598,7 +622,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>2</v>
       </c>
@@ -612,7 +636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>30</v>
       </c>
@@ -623,12 +647,40 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
         <v>8</v>
       </c>
       <c r="F10" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" t="s">
+        <v>35</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
check const and record for initialization
</commit_message>
<xml_diff>
--- a/test/module-xlsx/table.xlsx
+++ b/test/module-xlsx/table.xlsx
@@ -177,9 +177,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -484,7 +485,7 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -646,6 +647,9 @@
       <c r="F9" t="s">
         <v>31</v>
       </c>
+      <c r="G9">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
@@ -665,6 +669,9 @@
       <c r="F11" t="s">
         <v>35</v>
       </c>
+      <c r="J11">
+        <v>12</v>
+      </c>
       <c r="L11">
         <v>1</v>
       </c>
@@ -681,6 +688,9 @@
       </c>
       <c r="F12" t="s">
         <v>39</v>
+      </c>
+      <c r="J12" s="2">
+        <v>9.9000000000000005E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug fix in XLSX module
</commit_message>
<xml_diff>
--- a/test/module-xlsx/table.xlsx
+++ b/test/module-xlsx/table.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F5E1D5-1F65-483F-91D8-4615D308DF33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
   <si>
     <t>on</t>
   </si>
@@ -136,12 +137,21 @@
   </si>
   <si>
     <t>c1</t>
+  </si>
+  <si>
+    <t>aux.pmid[]</t>
+  </si>
+  <si>
+    <t>1111;</t>
+  </si>
+  <si>
+    <t>123;321</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -191,6 +201,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -238,7 +251,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -271,9 +284,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -306,6 +336,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -481,22 +528,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7265625" customWidth="1"/>
-    <col min="8" max="8" width="12.1796875" customWidth="1"/>
-    <col min="9" max="9" width="16.7265625" customWidth="1"/>
-    <col min="10" max="10" width="19.81640625" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" customWidth="1"/>
+    <col min="8" max="8" width="12.21875" customWidth="1"/>
+    <col min="9" max="9" width="16.77734375" customWidth="1"/>
+    <col min="10" max="10" width="19.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -533,8 +580,11 @@
       <c r="M1" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>1</v>
       </c>
@@ -545,7 +595,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -577,7 +627,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>0</v>
       </c>
@@ -603,7 +653,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>1</v>
       </c>
@@ -623,7 +673,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>2</v>
       </c>
@@ -637,7 +687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>30</v>
       </c>
@@ -651,7 +701,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>8</v>
       </c>
@@ -659,7 +709,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>1</v>
       </c>
@@ -678,8 +728,11 @@
       <c r="M11" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>1</v>
       </c>
@@ -691,6 +744,9 @@
       </c>
       <c r="J12" s="2">
         <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="N12" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -699,16 +755,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -731,7 +787,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -761,12 +817,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
table numeration from 0
</commit_message>
<xml_diff>
--- a/test/module-xlsx/table.xlsx
+++ b/test/module-xlsx/table.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F5E1D5-1F65-483F-91D8-4615D308DF33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C33528-AA8E-475B-8897-80413D8E8C8B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -531,7 +531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
@@ -758,8 +758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -804,7 +804,7 @@
         <v>19</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <v>5</v>

</xml_diff>